<commit_message>
Cleaned variables + calculations + Rstudio script
</commit_message>
<xml_diff>
--- a/Cleaned variables/paymentsPC_TOR_cleaned.xlsx
+++ b/Cleaned variables/paymentsPC_TOR_cleaned.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>PaymentIndex</t>
   </si>
@@ -27,6 +27,12 @@
   </si>
   <si>
     <t>TransactionValue</t>
+  </si>
+  <si>
+    <t>TransactionSpeedNS</t>
+  </si>
+  <si>
+    <t>TransactionSpeedMS</t>
   </si>
   <si>
     <t>1</t>
@@ -244,10 +250,16 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>69.0</v>
@@ -264,10 +276,16 @@
       <c r="F2" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G2" t="n">
+        <v>2.471182336E9</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2471.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>70.0</v>
@@ -284,10 +302,16 @@
       <c r="F3" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G3" t="n">
+        <v>2.4261056E9</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2426.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>71.0</v>
@@ -304,10 +328,16 @@
       <c r="F4" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G4" t="n">
+        <v>2.532618752E9</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2533.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>72.0</v>
@@ -324,10 +354,16 @@
       <c r="F5" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G5" t="n">
+        <v>2.777951488E9</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2778.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>73.0</v>
@@ -344,10 +380,16 @@
       <c r="F6" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G6" t="n">
+        <v>2.305387008E9</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2305.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>74.0</v>
@@ -364,10 +406,16 @@
       <c r="F7" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G7" t="n">
+        <v>2.458844672E9</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2459.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>75.0</v>
@@ -384,10 +432,16 @@
       <c r="F8" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G8" t="n">
+        <v>2.54750976E9</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2548.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>76.0</v>
@@ -404,10 +458,16 @@
       <c r="F9" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G9" t="n">
+        <v>3.17995904E9</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3180.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>77.0</v>
@@ -424,10 +484,16 @@
       <c r="F10" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G10" t="n">
+        <v>2.479346176E9</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2479.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>78.0</v>
@@ -444,10 +510,16 @@
       <c r="F11" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G11" t="n">
+        <v>2.39524736E9</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2395.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>79.0</v>
@@ -464,10 +536,16 @@
       <c r="F12" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G12" t="n">
+        <v>2.490301696E9</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2490.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>80.0</v>
@@ -484,10 +562,16 @@
       <c r="F13" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G13" t="n">
+        <v>2.553577984E9</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2554.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>81.0</v>
@@ -504,10 +588,16 @@
       <c r="F14" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G14" t="n">
+        <v>2.27576832E9</v>
+      </c>
+      <c r="H14" t="n">
+        <v>2276.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>82.0</v>
@@ -524,10 +614,16 @@
       <c r="F15" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G15" t="n">
+        <v>3.012856832E9</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3013.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>83.0</v>
@@ -544,10 +640,16 @@
       <c r="F16" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G16" t="n">
+        <v>2.82851712E9</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2829.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>84.0</v>
@@ -564,10 +666,16 @@
       <c r="F17" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G17" t="n">
+        <v>2.683521536E9</v>
+      </c>
+      <c r="H17" t="n">
+        <v>2684.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>85.0</v>
@@ -584,10 +692,16 @@
       <c r="F18" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G18" t="n">
+        <v>2.446162944E9</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2446.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>86.0</v>
@@ -604,10 +718,16 @@
       <c r="F19" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G19" t="n">
+        <v>3.266533376E9</v>
+      </c>
+      <c r="H19" t="n">
+        <v>3267.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>87.0</v>
@@ -624,10 +744,16 @@
       <c r="F20" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G20" t="n">
+        <v>2.658136832E9</v>
+      </c>
+      <c r="H20" t="n">
+        <v>2658.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>88.0</v>
@@ -644,10 +770,16 @@
       <c r="F21" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G21" t="n">
+        <v>2.852175104E9</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2852.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>89.0</v>
@@ -664,10 +796,16 @@
       <c r="F22" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G22" t="n">
+        <v>2.277335808E9</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2277.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>90.0</v>
@@ -684,10 +822,16 @@
       <c r="F23" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G23" t="n">
+        <v>2.297745152E9</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2298.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>91.0</v>
@@ -704,10 +848,16 @@
       <c r="F24" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G24" t="n">
+        <v>2.362645504E9</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2363.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B25" t="n">
         <v>92.0</v>
@@ -724,10 +874,16 @@
       <c r="F25" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G25" t="n">
+        <v>2.638869248E9</v>
+      </c>
+      <c r="H25" t="n">
+        <v>2639.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B26" t="n">
         <v>93.0</v>
@@ -744,10 +900,16 @@
       <c r="F26" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G26" t="n">
+        <v>2.520755968E9</v>
+      </c>
+      <c r="H26" t="n">
+        <v>2521.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B27" t="n">
         <v>94.0</v>
@@ -764,10 +926,16 @@
       <c r="F27" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G27" t="n">
+        <v>2.527098368E9</v>
+      </c>
+      <c r="H27" t="n">
+        <v>2527.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B28" t="n">
         <v>95.0</v>
@@ -784,10 +952,16 @@
       <c r="F28" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G28" t="n">
+        <v>2.476846848E9</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2477.0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B29" t="n">
         <v>96.0</v>
@@ -804,10 +978,16 @@
       <c r="F29" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G29" t="n">
+        <v>2.98783488E9</v>
+      </c>
+      <c r="H29" t="n">
+        <v>2988.0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B30" t="n">
         <v>97.0</v>
@@ -824,10 +1004,16 @@
       <c r="F30" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G30" t="n">
+        <v>2.424101376E9</v>
+      </c>
+      <c r="H30" t="n">
+        <v>2424.0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B31" t="n">
         <v>98.0</v>
@@ -844,10 +1030,16 @@
       <c r="F31" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G31" t="n">
+        <v>2.50489856E9</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2505.0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B32" t="n">
         <v>99.0</v>
@@ -864,10 +1056,16 @@
       <c r="F32" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G32" t="n">
+        <v>2.639440896E9</v>
+      </c>
+      <c r="H32" t="n">
+        <v>2639.0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B33" t="n">
         <v>100.0</v>
@@ -884,10 +1082,16 @@
       <c r="F33" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G33" t="n">
+        <v>2.388601344E9</v>
+      </c>
+      <c r="H33" t="n">
+        <v>2389.0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B34" t="n">
         <v>101.0</v>
@@ -904,10 +1108,16 @@
       <c r="F34" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G34" t="n">
+        <v>2.375588608E9</v>
+      </c>
+      <c r="H34" t="n">
+        <v>2376.0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B35" t="n">
         <v>102.0</v>
@@ -924,10 +1134,16 @@
       <c r="F35" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G35" t="n">
+        <v>2.443535872E9</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2444.0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B36" t="n">
         <v>103.0</v>
@@ -944,10 +1160,16 @@
       <c r="F36" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G36" t="n">
+        <v>2.360035584E9</v>
+      </c>
+      <c r="H36" t="n">
+        <v>2360.0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B37" t="n">
         <v>104.0</v>
@@ -964,10 +1186,16 @@
       <c r="F37" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G37" t="n">
+        <v>2.285167104E9</v>
+      </c>
+      <c r="H37" t="n">
+        <v>2285.0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B38" t="n">
         <v>105.0</v>
@@ -984,10 +1212,16 @@
       <c r="F38" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G38" t="n">
+        <v>2.424911104E9</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2425.0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B39" t="n">
         <v>106.0</v>
@@ -1004,10 +1238,16 @@
       <c r="F39" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G39" t="n">
+        <v>2.439161856E9</v>
+      </c>
+      <c r="H39" t="n">
+        <v>2439.0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B40" t="n">
         <v>107.0</v>
@@ -1024,10 +1264,16 @@
       <c r="F40" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G40" t="n">
+        <v>2.501559296E9</v>
+      </c>
+      <c r="H40" t="n">
+        <v>2502.0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B41" t="n">
         <v>108.0</v>
@@ -1044,10 +1290,16 @@
       <c r="F41" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G41" t="n">
+        <v>2.318461696E9</v>
+      </c>
+      <c r="H41" t="n">
+        <v>2318.0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B42" t="n">
         <v>109.0</v>
@@ -1064,10 +1316,16 @@
       <c r="F42" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G42" t="n">
+        <v>2.553885952E9</v>
+      </c>
+      <c r="H42" t="n">
+        <v>2554.0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B43" t="n">
         <v>110.0</v>
@@ -1084,10 +1342,16 @@
       <c r="F43" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G43" t="n">
+        <v>2.33369344E9</v>
+      </c>
+      <c r="H43" t="n">
+        <v>2334.0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B44" t="n">
         <v>111.0</v>
@@ -1104,10 +1368,16 @@
       <c r="F44" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G44" t="n">
+        <v>2.551133696E9</v>
+      </c>
+      <c r="H44" t="n">
+        <v>2551.0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B45" t="n">
         <v>112.0</v>
@@ -1124,10 +1394,16 @@
       <c r="F45" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G45" t="n">
+        <v>2.484172544E9</v>
+      </c>
+      <c r="H45" t="n">
+        <v>2484.0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B46" t="n">
         <v>113.0</v>
@@ -1144,10 +1420,16 @@
       <c r="F46" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G46" t="n">
+        <v>2.605879296E9</v>
+      </c>
+      <c r="H46" t="n">
+        <v>2606.0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B47" t="n">
         <v>114.0</v>
@@ -1164,10 +1446,16 @@
       <c r="F47" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G47" t="n">
+        <v>2.741762304E9</v>
+      </c>
+      <c r="H47" t="n">
+        <v>2742.0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B48" t="n">
         <v>115.0</v>
@@ -1184,10 +1472,16 @@
       <c r="F48" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G48" t="n">
+        <v>2.273619456E9</v>
+      </c>
+      <c r="H48" t="n">
+        <v>2274.0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B49" t="n">
         <v>116.0</v>
@@ -1204,10 +1498,16 @@
       <c r="F49" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G49" t="n">
+        <v>2.444374784E9</v>
+      </c>
+      <c r="H49" t="n">
+        <v>2444.0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B50" t="n">
         <v>117.0</v>
@@ -1224,10 +1524,16 @@
       <c r="F50" t="n">
         <v>1500.0</v>
       </c>
+      <c r="G50" t="n">
+        <v>2.535765248E9</v>
+      </c>
+      <c r="H50" t="n">
+        <v>2536.0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B51" t="n">
         <v>118.0</v>
@@ -1243,6 +1549,12 @@
       </c>
       <c r="F51" t="n">
         <v>1500.0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>2.466799104E9</v>
+      </c>
+      <c r="H51" t="n">
+        <v>2467.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>